<commit_message>
add id_posyandu to input excel
</commit_message>
<xml_diff>
--- a/storage/app/contoh_excel/input_data.xlsx
+++ b/storage/app/contoh_excel/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\File Rasyad\Career\Projects\sipi-all\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3834414-E966-4027-A965-4023A7110FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0DAB5A-0646-45C3-ABBA-3A7995AC632F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{64992207-49C9-4619-A350-C1574D8FA26E}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11505" xr2:uid="{64992207-49C9-4619-A350-C1574D8FA26E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>id_antigen</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>id_anak</t>
+  </si>
+  <si>
+    <t>id_posyandu</t>
   </si>
 </sst>
 </file>
@@ -107,13 +110,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2EEFB69A-52DC-4150-A900-2AFC2AA78CE9}" name="Table1" displayName="Table1" ref="A1:D31" totalsRowShown="0">
-  <autoFilter ref="A1:D31" xr:uid="{2EEFB69A-52DC-4150-A900-2AFC2AA78CE9}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2EEFB69A-52DC-4150-A900-2AFC2AA78CE9}" name="Table1" displayName="Table1" ref="A1:E31" totalsRowShown="0">
+  <autoFilter ref="A1:E31" xr:uid="{2EEFB69A-52DC-4150-A900-2AFC2AA78CE9}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{3970CE30-FECB-4FE4-91D1-17199AF8921D}" name="no"/>
     <tableColumn id="2" xr3:uid="{DA66010D-4E0E-4569-B8D9-3F3CD013B594}" name="id_anak"/>
     <tableColumn id="3" xr3:uid="{8DADB2B3-3F64-4CE4-8A62-0ACD852CB630}" name="id_antigen"/>
     <tableColumn id="4" xr3:uid="{098EE7B4-24B8-4001-B14F-C750AAC41E00}" name="tanggal_pemberian" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{1A3F834A-06EB-4F86-99F1-2F00BC8A4ACA}" name="id_posyandu"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -416,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C7E81FA-172F-4C70-8042-27CCD23110B7}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +434,7 @@
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -443,8 +447,11 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -457,86 +464,89 @@
       <c r="D2" s="1">
         <v>44196</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>